<commit_message>
add product name in urdu in prroduct
</commit_message>
<xml_diff>
--- a/public/product.xlsx
+++ b/public/product.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <definedNames/>
+  <calcPr fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="17">
   <si>
     <t>id</t>
   </si>
@@ -59,14 +60,34 @@
   </si>
   <si>
     <t>2025-04-15</t>
+  </si>
+  <si>
+    <t>namInUrdu</t>
+  </si>
+  <si>
+    <t>urdu</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+  <fonts count="4">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -76,10 +97,9 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -111,23 +131,128 @@
       <bottom style="thin">
         <color auto="1"/>
       </bottom>
-      <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+  <cellStyleXfs count="20">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
+      <alignment/>
+      <protection/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top"/>
+      <protection/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="15" builtinId="5"/>
+    <cellStyle name="Currency" xfId="16" builtinId="4"/>
+    <cellStyle name="Currency [0]" xfId="17" builtinId="7"/>
+    <cellStyle name="Comma" xfId="18" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="19" builtinId="6"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -415,91 +540,102 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:J3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0" topLeftCell="A1">
+      <selection pane="topLeft" activeCell="C5" sqref="C5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:9">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:10" ht="15" customHeight="1">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:10" ht="15">
       <c r="A2" t="s">
         <v>9</v>
       </c>
       <c r="B2" t="s">
         <v>10</v>
       </c>
-      <c r="D2" t="s">
+      <c r="C2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E2" t="s">
         <v>11</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>13</v>
       </c>
-      <c r="F2">
+      <c r="G2">
         <v>200</v>
       </c>
-      <c r="G2">
+      <c r="H2">
         <v>250</v>
       </c>
-      <c r="H2">
+      <c r="I2">
         <v>300</v>
       </c>
-      <c r="I2">
+      <c r="J2">
         <v>99</v>
       </c>
     </row>
-    <row r="3" spans="1:9">
+    <row r="3" spans="1:10" ht="15">
       <c r="A3" t="s">
         <v>9</v>
       </c>
       <c r="B3" t="s">
         <v>10</v>
       </c>
-      <c r="D3" t="s">
+      <c r="C3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E3" t="s">
         <v>12</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>14</v>
       </c>
-      <c r="F3">
+      <c r="G3">
         <v>220</v>
       </c>
-      <c r="G3">
+      <c r="H3">
         <v>270</v>
       </c>
-      <c r="H3">
+      <c r="I3">
         <v>320</v>
       </c>
-      <c r="I3">
+      <c r="J3">
         <v>50</v>
       </c>
     </row>

</xml_diff>